<commit_message>
Add moving averages to demographic datasets
</commit_message>
<xml_diff>
--- a/etl/data/input/Datos_carga_mensual_demo.xlsx
+++ b/etl/data/input/Datos_carga_mensual_demo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Defunciones meses" sheetId="1" state="visible" r:id="rId2"/>
@@ -638,8 +638,8 @@
   </sheetPr>
   <dimension ref="A1:AB19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M20" activeCellId="0" sqref="M20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2432,7 +2432,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3105,8 +3105,8 @@
   </sheetPr>
   <dimension ref="A1:CJ18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BR1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BS2" activeCellId="0" sqref="BS2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AB1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AL1" activeCellId="0" sqref="AL1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6886,7 +6886,7 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S16" activeCellId="0" sqref="S16"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9908,7 +9908,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>